<commit_message>
exports no longer have the pandas labels
</commit_message>
<xml_diff>
--- a/Items_Markup.xlsx
+++ b/Items_Markup.xlsx
@@ -812,7 +812,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1" activeCellId="0"/>
+      <selection pane="topRight" activeCell="E8" sqref="E8" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" defaultColWidth="8.88671875" outlineLevelCol="0"/>
@@ -1078,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
@@ -2054,7 +2054,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" ht="28">
+    <row r="34" ht="27">
       <c r="A34" s="1">
         <f>A33+1</f>
         <v>26</v>
@@ -2120,7 +2120,7 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
-    <row r="36" ht="86">
+    <row r="36" ht="85">
       <c r="A36" s="1">
         <f>A35+1</f>
         <v>28</v>
@@ -2180,7 +2180,7 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
-    <row r="38" ht="100">
+    <row r="38" ht="99">
       <c r="A38" s="1">
         <f>A37+1</f>
         <v>30</v>
@@ -2210,7 +2210,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
-    <row r="39" ht="28">
+    <row r="39" ht="27">
       <c r="A39" s="1">
         <f>A38+1</f>
         <v>31</v>
@@ -2240,7 +2240,7 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
     </row>
-    <row r="40" ht="28">
+    <row r="40" ht="27">
       <c r="A40" s="1">
         <f>A39+1</f>
         <v>32</v>

</xml_diff>